<commit_message>
change passive properties paradigm
</commit_message>
<xml_diff>
--- a/data/L5/multicomp_coefs.xlsx
+++ b/data/L5/multicomp_coefs.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladimiromelyusik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladimiromelyusik/ACT/data/L5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{706D1654-A1D7-464F-A41F-3E970F9CC2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77489DA6-8322-8144-8675-D48C521C6C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{F510DF22-169C-EF40-BBDA-032EC062BC36}"/>
+    <workbookView xWindow="10360" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{F510DF22-169C-EF40-BBDA-032EC062BC36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,23 +507,20 @@
         <v>5.8900000000000002E-5</v>
       </c>
       <c r="D2" s="1">
-        <f>B2/C2</f>
-        <v>0.57385398981324276</v>
+        <f>C2/B2</f>
+        <v>1.7426035502958579</v>
       </c>
       <c r="E2">
         <v>4.6699999999999997E-5</v>
       </c>
       <c r="F2" s="1">
-        <f>B2/E2</f>
-        <v>0.72376873661670249</v>
+        <f>E2/B2</f>
+        <v>1.3816568047337277</v>
       </c>
       <c r="G2">
         <v>3.2499999999999997E-5</v>
       </c>
-      <c r="H2" s="1">
-        <f>B2/G2</f>
-        <v>1.04</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -558,15 +555,15 @@
         <v>2.61E-4</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D3:D11" si="0">B5/C5</f>
-        <v>2655.1724137931033</v>
+        <f t="shared" ref="D3:D11" si="0">C5/B5</f>
+        <v>3.7662337662337667E-4</v>
       </c>
       <c r="E5">
         <v>2.61E-4</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F3:F11" si="1">B5/E5</f>
-        <v>2655.1724137931033</v>
+        <f t="shared" ref="F3:F11" si="1">E5/B5</f>
+        <v>3.7662337662337667E-4</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -616,7 +613,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>31.924882629107984</v>
+        <v>3.1323529411764701E-2</v>
       </c>
       <c r="E9">
         <f>3*0.0213</f>
@@ -624,7 +621,7 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>31.924882629107984</v>
+        <v>3.1323529411764701E-2</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -640,7 +637,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0.05</v>
       </c>
       <c r="E10">
         <v>2.0000000000000001E-4</v>
@@ -658,17 +655,11 @@
       <c r="C11">
         <v>6.7500000000000001E-5</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11">
         <v>6.7500000000000001E-5</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="H11" s="1"/>
     </row>
   </sheetData>

</xml_diff>